<commit_message>
primera prueba de migracion de ingresos completada
</commit_message>
<xml_diff>
--- a/app/db_models/CuentasEfectivo.xlsx
+++ b/app/db_models/CuentasEfectivo.xlsx
@@ -2,59 +2,232 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abazbaz/R2/app/db_models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C300E8F2-E436-3F4F-9CEA-952F1F1FFC10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DD6F91-6264-9947-BA74-75C2CCC12FC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-400" yWindow="1280" windowWidth="25600" windowHeight="14560" xr2:uid="{FE86E832-6114-4F74-B5CA-82A3579B7E8E}"/>
+    <workbookView xWindow="3080" yWindow="460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Centro de Negocios Nombre</t>
-  </si>
-  <si>
-    <t>Cuenta Efectivo 1</t>
-  </si>
-  <si>
-    <t>Cuenta Efectivo 2</t>
-  </si>
-  <si>
-    <t># de Sucursal (Sucnsucursal en Gez)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>SAN JUAN 1</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>TAF -2  100156</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>R U D O S  -  CENTRO</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>R  U  D  O  S  - COAPA</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>SAN JUAN 2 (CIRCUNVALACION 1)</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>TAF-6 100209</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>R  U  D  O  S  - BUENAVISTA</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>R U D O S - PLAZA LA ROSA</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>R  U  D  O  S  - TEPEYAC</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>TAF -11  100317</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>TAF-12 100277</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>RUDOS ARAGON</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>TAF-14 100147</t>
+  </si>
+  <si>
+    <t>014</t>
+  </si>
+  <si>
+    <t>R  U  D  O  S  - LINDAVISTA</t>
+  </si>
+  <si>
+    <t>015</t>
+  </si>
+  <si>
+    <t>RUDOS "MORELIA"</t>
+  </si>
+  <si>
+    <t>016</t>
+  </si>
+  <si>
+    <t>RUDOS - VALLEJO</t>
+  </si>
+  <si>
+    <t>017</t>
+  </si>
+  <si>
+    <t>RUDOS XALAPA</t>
+  </si>
+  <si>
+    <t>018</t>
+  </si>
+  <si>
+    <t>R  U  D  O  S  - SATELITE</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>R U D O S  - SANTA FE</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>RUDOS  - LAS AMERICAS</t>
+  </si>
+  <si>
+    <t>021</t>
+  </si>
+  <si>
+    <t>RUDOS TEZONTLE</t>
+  </si>
+  <si>
+    <t>022</t>
+  </si>
+  <si>
+    <t>RUDOS - PLAZA SAN MIGUEL</t>
+  </si>
+  <si>
+    <t>024</t>
+  </si>
+  <si>
+    <t>RUDOS -  TEXCOCO</t>
+  </si>
+  <si>
+    <t>025</t>
+  </si>
+  <si>
+    <t>RUDOS - PARQUE DELTA</t>
+  </si>
+  <si>
+    <t>027</t>
+  </si>
+  <si>
+    <t>RUDOS - C.D JARDIN</t>
+  </si>
+  <si>
+    <t>028</t>
+  </si>
+  <si>
+    <t>numer_sucursal</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>efectivo_1</t>
+  </si>
+  <si>
+    <t>efectivo_2</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>055637</t>
+  </si>
+  <si>
+    <t>0103783111</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,28 +251,39 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -411,59 +595,455 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A9607E4-77C2-4FE7-A541-3EE33D5A66E2}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
     <col min="3" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B40" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>